<commit_message>
Change Index value to show correct no of login
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="14360" windowHeight="4620"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="14355" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -924,18 +924,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.7265625" customWidth="1"/>
-    <col min="4" max="4" width="40.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -971,7 +971,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -982,7 +982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -993,7 +993,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>8</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>9</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>9</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>10</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>11</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>12</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>12</v>
       </c>
@@ -1458,11 +1458,11 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1478,13 +1478,13 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="122.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>15</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>17</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>19</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>25</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>27</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>31</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>33</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>35</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>37</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>43</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>45</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>47</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>49</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>51</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>53</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>55</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>57</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>59</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>61</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>63</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>65</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>67</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>69</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>71</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>73</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>75</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>77</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>79</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>81</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>83</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>85</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>87</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>89</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>91</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>93</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>95</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>97</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>99</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
[Scale] modified database file
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="14355" windowHeight="4620"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="14360" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="187">
   <si>
     <t>Field</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>chatID</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t xml:space="preserve">You may login to the application by using the user name and password provided by the compliance SPOC of your company. </t>
   </si>
   <si>
-    <t xml:space="preserve">Contact the compliance SPOC of your company or write an email to compliance.support@in.ey.com. </t>
-  </si>
-  <si>
     <t xml:space="preserve">	Line 17: •	Q</t>
   </si>
   <si>
@@ -580,6 +574,9 @@
   </si>
   <si>
     <t>Whom do I contact in case of any legal query?</t>
+  </si>
+  <si>
+    <t>Contact the compliance SPOC of your company or write an email to compliance.support@in.ey.com.</t>
   </si>
 </sst>
 </file>
@@ -922,526 +919,523 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.7265625" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B33" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
+      <c r="C39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
+      <c r="B40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
+      <c r="B42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D42" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D46" t="s">
-        <v>103</v>
+      <c r="C46" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1458,11 +1452,11 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1478,362 +1472,362 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="122.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
         <v>59</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
         <v>61</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
         <v>63</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
         <v>65</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
         <v>71</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
         <v>75</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
         <v>77</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
         <v>79</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
         <v>81</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
         <v>83</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
         <v>85</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
         <v>87</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
         <v>89</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
         <v>91</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
         <v>93</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
         <v>95</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
         <v>97</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
         <v>99</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Sample Deploy question answer update]
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="199">
   <si>
     <t>Field</t>
   </si>
@@ -474,15 +474,6 @@
     <t>Which report do I download to view all the compliances already submitted?</t>
   </si>
   <si>
-    <t>How do I login to the application?</t>
-  </si>
-  <si>
-    <t>What are the different types of authentication mechanisms used by the compliance manager application?</t>
-  </si>
-  <si>
-    <t>From where do I get the URL of the compliance manager application?</t>
-  </si>
-  <si>
     <t>How do I view my task list as an owner?</t>
   </si>
   <si>
@@ -495,24 +486,6 @@
     <t>Who all have the view to the compliance To Do List?</t>
   </si>
   <si>
-    <t>What does an owner do?</t>
-  </si>
-  <si>
-    <t>What does an approver do?</t>
-  </si>
-  <si>
-    <t>What does a reviewer do?</t>
-  </si>
-  <si>
-    <t>What does an auditor do?</t>
-  </si>
-  <si>
-    <t>What does a location owner do?</t>
-  </si>
-  <si>
-    <t>What does an administrator do?</t>
-  </si>
-  <si>
     <t>How do I approve compliances as an approver?</t>
   </si>
   <si>
@@ -577,6 +550,69 @@
   </si>
   <si>
     <t>Contact the compliance SPOC of your company or write an email to compliance.support@in.ey.com.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">different type authentication mechanisms used compliance manager application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">type authentication mechanisms used compliance manager application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">different authentication mechanisms used compliance manager application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">type authentication mechanisms </t>
+  </si>
+  <si>
+    <t xml:space="preserve">different authentication mechanisms </t>
+  </si>
+  <si>
+    <t xml:space="preserve">get URL compliance manager application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL compliance manager application </t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>auditor</t>
+  </si>
+  <si>
+    <t>reviewer</t>
+  </si>
+  <si>
+    <t>location owner</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>Appointment of dealer</t>
+  </si>
+  <si>
+    <t>What is the process for appointment of dealer?</t>
+  </si>
+  <si>
+    <t>Whoes approval is required?</t>
+  </si>
+  <si>
+    <t>First approval by Area head and final approval by Head of Sales.</t>
+  </si>
+  <si>
+    <t>Download form</t>
+  </si>
+  <si>
+    <t>Please clink on this link (Template 1).</t>
+  </si>
+  <si>
+    <t>You need to fill dealer appointment form, obtain requsite approvals.</t>
   </si>
 </sst>
 </file>
@@ -919,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,98 +984,98 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" t="s">
-        <v>136</v>
+        <v>184</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1047,10 +1083,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1058,10 +1094,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1069,10 +1105,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1080,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1091,76 +1127,76 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1168,10 +1204,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1179,10 +1215,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1190,10 +1226,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1201,10 +1237,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1212,10 +1248,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1223,10 +1259,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1234,208 +1270,307 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "test 2 modified"
This reverts commit 6516b5bc617ce45a3b1cc64ebf027f2140ed5ebf.
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chirag1.gupta\EnYchatbot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9740"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="3" r:id="rId1"/>
@@ -62,6 +57,9 @@
     <t>Who is responsible for creation of business partner code ?</t>
   </si>
   <si>
+    <t>How do we appoint business partner ?</t>
+  </si>
+  <si>
     <t>Who is responsible for preparing performance report of business partner ?</t>
   </si>
   <si>
@@ -242,6 +240,9 @@
     <t>On what basis rates of handling agent are decided ?</t>
   </si>
   <si>
+    <t>State Head shall perform ‘Need Assessment’ and submit the same to CMO for review.</t>
+  </si>
+  <si>
     <t xml:space="preserve">State Head shall be responsible for identification of business partner </t>
   </si>
   <si>
@@ -417,12 +418,6 @@
   </si>
   <si>
     <t>Dealer Registration</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>Test 4</t>
   </si>
 </sst>
 </file>
@@ -768,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -778,697 +773,697 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FaQSheet answers spaces modify]
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -336,9 +336,6 @@
     <t>Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Please refer Working template 1 </t>
-  </si>
-  <si>
     <t>Please refer Working template 2</t>
   </si>
   <si>
@@ -418,6 +415,9 @@
   </si>
   <si>
     <t>Dealer Registration</t>
+  </si>
+  <si>
+    <t>Please refer Working template 1</t>
   </si>
 </sst>
 </file>
@@ -763,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,15 +789,15 @@
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -830,29 +830,29 @@
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -863,18 +863,18 @@
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -924,12 +924,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -940,18 +940,18 @@
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>81</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>83</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>85</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>87</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>89</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>91</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>93</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>95</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>96</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>98</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>100</v>
@@ -1072,13 +1072,13 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1089,7 +1089,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1111,7 +1111,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1119,10 +1119,10 @@
         <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1133,7 +1133,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1141,10 +1141,10 @@
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1155,7 +1155,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1182,7 +1182,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>43</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>16</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
@@ -1243,7 +1243,7 @@
         <v>71</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1254,7 +1254,7 @@
         <v>19</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1276,12 +1276,12 @@
         <v>20</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>24</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>21</v>
@@ -1303,13 +1303,13 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1339,7 +1339,7 @@
         <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Added one line - chirag
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chirag1.gupta\EnYchatbot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="3" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
   <si>
     <t>What is the pre requisite for appointment of business partner ?</t>
   </si>
@@ -418,6 +423,21 @@
   </si>
   <si>
     <t>Please refer Working template 1</t>
+  </si>
+  <si>
+    <t>Client Requisition</t>
+  </si>
+  <si>
+    <t>What are the type of projects that CPWD can receive a requisition for?</t>
+  </si>
+  <si>
+    <t>1. Construction
+    a. New work (Civil, Electrical, Horticulture)
+    b. Upgradation work (Civil, Electrical, Horticulture)
+2. Maintenance
+    a. Day to day repair 
+    b. Annual repair 
+    c. Special repair</t>
   </si>
 </sst>
 </file>
@@ -474,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -491,6 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -771,20 +792,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.54296875" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>103</v>
       </c>
@@ -795,7 +814,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>121</v>
       </c>
@@ -806,7 +825,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -817,7 +836,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
@@ -828,7 +847,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -839,7 +858,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
@@ -850,7 +869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
@@ -861,7 +880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>121</v>
       </c>
@@ -872,7 +891,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
@@ -883,7 +902,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -894,7 +913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -905,7 +924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>122</v>
       </c>
@@ -916,7 +935,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
@@ -927,7 +946,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -938,7 +957,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>123</v>
       </c>
@@ -960,7 +979,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>130</v>
       </c>
@@ -971,7 +990,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -1004,7 +1023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>122</v>
       </c>
@@ -1015,7 +1034,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -1026,7 +1045,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>123</v>
       </c>
@@ -1037,7 +1056,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
@@ -1048,7 +1067,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -1059,7 +1078,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>126</v>
       </c>
@@ -1070,7 +1089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
@@ -1081,7 +1100,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1111,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1103,7 +1122,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1114,7 +1133,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1125,7 +1144,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1136,7 +1155,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1166,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1177,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1199,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>119</v>
       </c>
@@ -1191,7 +1210,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>119</v>
       </c>
@@ -1202,7 +1221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>119</v>
       </c>
@@ -1213,7 +1232,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -1235,7 +1254,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1265,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -1257,7 +1276,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -1268,7 +1287,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -1279,7 +1298,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>120</v>
       </c>
@@ -1290,7 +1309,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>120</v>
       </c>
@@ -1301,7 +1320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>120</v>
       </c>
@@ -1312,7 +1331,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -1334,7 +1353,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1364,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1375,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>26</v>
       </c>
@@ -1367,7 +1386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>26</v>
       </c>
@@ -1378,7 +1397,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1408,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
@@ -1400,7 +1419,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>32</v>
       </c>
@@ -1411,7 +1430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>32</v>
       </c>
@@ -1422,7 +1441,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>32</v>
       </c>
@@ -1433,7 +1452,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>32</v>
       </c>
@@ -1444,7 +1463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1474,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>32</v>
       </c>
@@ -1464,6 +1483,17 @@
       </c>
       <c r="C62" s="1" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/FaQSheet.xlsx
+++ b/FaQSheet.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1'!$A$1:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
   <si>
     <t>What is the pre requisite for appointment of business partner ?</t>
   </si>
@@ -438,6 +438,66 @@
     a. Day to day repair 
     b. Annual repair 
     c. Special repair</t>
+  </si>
+  <si>
+    <t>What mode will a construction project be executed on ?</t>
+  </si>
+  <si>
+    <t>Geographical mode (&lt;100 crores) or Project mode (&gt;100 crores or important client or project)</t>
+  </si>
+  <si>
+    <t>Is there any exception to team composition in a Project Mode assignment ?</t>
+  </si>
+  <si>
+    <t>Decision to form a separate team is also taken by Director General (DG) CPWD considering the parameters like the work load, quantum of work, availability staff etc.</t>
+  </si>
+  <si>
+    <t>Who should be the Executing Engineer/Office for a project?</t>
+  </si>
+  <si>
+    <t>If Geographical mode, concerned Division office/Circle Office/Zonal Office in the geographical jurisdiction
+If Project Mode, Project Manager (PM) or Chief Project Manager (CPM)</t>
+  </si>
+  <si>
+    <t>What is team composition for a Project Mode assignment ?</t>
+  </si>
+  <si>
+    <t>Who are our clients?</t>
+  </si>
+  <si>
+    <t>What is the basis of deciding Competent Authority for any approval ?</t>
+  </si>
+  <si>
+    <t>Competent Authority is decided as per the Delegation of Financial Powers (DFPR) as mentioned in Table A</t>
+  </si>
+  <si>
+    <t>PM/CPM, EE, AE, AEE and JE</t>
+  </si>
+  <si>
+    <t>The clientele can be categorized as follows :- 
+1. Ministry of GoI (leading to Budgeted and Authorised Works)
+2. Autonomous bodies (leading to Deposit Works) 
+3. PSU's (leading to Deposit Works) 
+4. NGO's (leading to Deposit Works) 
+5. Private organization (leading to Deposit Works)</t>
+  </si>
+  <si>
+    <t>Preliminary estimates (PE)</t>
+  </si>
+  <si>
+    <t>Administrative approvals and expenditure sanction</t>
+  </si>
+  <si>
+    <t>Detailed estimates</t>
+  </si>
+  <si>
+    <t>Technical sanction</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
 </sst>
 </file>
@@ -792,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C63"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,6 +1558,116 @@
         <v>134</v>
       </c>
     </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>